<commit_message>
- Berechtigungskonzept hinzugefügt - EPKs aktualsiert - UseCase aktualsiert - Systemübersichten hinzugefügt - Pflichtenheft aktualsiert
</commit_message>
<xml_diff>
--- a/documents/backend/Berechtigungskonzept_PAMS.xlsx
+++ b/documents/backend/Berechtigungskonzept_PAMS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5111b649650785fa/Dokumente/DHBW-Timo/4. Semester/PAMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Timo-\OneDrive\Dokumente\DHBW-Timo\4. Semester\PAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="28">
   <si>
     <t>Berechtigungskonzept PAMS</t>
   </si>
   <si>
-    <t>Anmelden</t>
-  </si>
-  <si>
     <t>Projektantrag erstellen</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>Bereichsleiter</t>
   </si>
   <si>
-    <t>Geschäftsführer</t>
-  </si>
-  <si>
     <t>Ja</t>
   </si>
   <si>
@@ -65,12 +59,6 @@
     <t>Gesamt-Budget einsehen</t>
   </si>
   <si>
-    <t>Projekte genehmigen/ablehnen (Final, Budget im Rahmen)</t>
-  </si>
-  <si>
-    <t>Projekte genehmigen/ablehnen (Final, Budget über Rahmen)</t>
-  </si>
-  <si>
     <t>Projektantrag bearbeiten (eigene)</t>
   </si>
   <si>
@@ -93,6 +81,33 @@
   </si>
   <si>
     <t>Projekte suchen (eigene)</t>
+  </si>
+  <si>
+    <t>Projekte genehmigen/ablehnen (Ebene 3)</t>
+  </si>
+  <si>
+    <t>Ebene 1: Formkontrolle - Sind alle nötigen Informationen vorhanden?</t>
+  </si>
+  <si>
+    <t>Ebene 2: Kennzahlen und Budget prüfung - Ist das Projekt Rentabel? Liegt das Budget unter 100.000,00€?</t>
+  </si>
+  <si>
+    <t>Standort- und Geschäftsleiter</t>
+  </si>
+  <si>
+    <t>Projekte genehmigen/ablehnen (Ebene 2.5, Budget über Rahmen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ebene 2.5: Budgetprüfung - Ist ein Budget von mehr als 100.000,00€ gerechtfertigt? </t>
+  </si>
+  <si>
+    <t>Ebene 3: Personalprüfung - Ist ausreichend Personal verfügbar?</t>
+  </si>
+  <si>
+    <t>Anmelden (Erst nach Freischaltung durch Vorgesetzten)</t>
+  </si>
+  <si>
+    <t>Mitarbeiter für PAMS freischalten</t>
   </si>
 </sst>
 </file>
@@ -182,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -238,6 +253,75 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -246,18 +330,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -267,6 +346,37 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20 % - Akzent5" xfId="2" builtinId="46"/>
@@ -549,353 +659,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="10" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>